<commit_message>
Added security in case some of the .txt files (msg,trusted) are deleted
</commit_message>
<xml_diff>
--- a/Codigos_Mensagens.xlsx
+++ b/Codigos_Mensagens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everlong\Google Drive\Faculdade\Segurança e Confiabilidade\Projecto\Trabalho 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DF70E1-3987-4954-9907-95E6350490D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E417DCBE-6AFC-400D-8AEF-FABE0B2AB4F6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>concluido não mexer na implementação</t>
   </si>
   <si>
-    <t>OP_ERROR or ERR_NOT_FRIENDS or ERR_NOT_REGISTERED</t>
-  </si>
-  <si>
     <t>OP_RES_ARRAY &lt;arrCode of ERR_YOURSELF or ERR_NOT_REGISTERED or ERR_ALREADY_EXISTS or OP_SUCCESSFUL&gt;</t>
   </si>
   <si>
@@ -129,13 +126,16 @@
     <t>OP_SUCCESSFUL &lt;byteArray&gt;</t>
   </si>
   <si>
-    <t>ERR_YOURSELF or ERR_NOT_FOUND or ERR_NOT_FRIENDS or ERR_NOT_REGISTERED</t>
-  </si>
-  <si>
     <t>Mensagem de pedido</t>
   </si>
   <si>
     <t>DOWNLOAD_FILE &lt;arrStr(fileOwner,fileName)&gt;</t>
+  </si>
+  <si>
+    <t>ERR_YOURSELF or ERR_NOT_FOUND or ERR_NOT_TRUSTED or ERR_NOT_REGISTERED</t>
+  </si>
+  <si>
+    <t>OP_ERROR or ERR_NOT_TRUSTED or ERR_NOT_REGISTERED</t>
   </si>
 </sst>
 </file>
@@ -404,6 +404,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -414,42 +450,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -734,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C7:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>9</v>
@@ -768,10 +768,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -783,7 +783,7 @@
         <v>17</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="22" t="s">
         <v>25</v>
       </c>
     </row>
@@ -798,7 +798,7 @@
         <v>16</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="11"/>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="6"/>
@@ -817,10 +817,10 @@
         <v>10</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="24" t="s">
         <v>23</v>
       </c>
     </row>
@@ -829,7 +829,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="12"/>
+      <c r="G13" s="24"/>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
@@ -851,7 +851,7 @@
         <v>17</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="25" t="s">
         <v>24</v>
       </c>
     </row>
@@ -863,10 +863,10 @@
         <v>12</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="13"/>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="6"/>
@@ -885,7 +885,7 @@
         <v>13</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -904,10 +904,10 @@
         <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="9"/>
@@ -916,7 +916,7 @@
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -938,7 +938,7 @@
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -951,7 +951,7 @@
         <v>18</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1000,197 +1000,197 @@
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D30" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="16" t="s">
+      <c r="D30" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>31</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="20"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="22" t="s">
+      <c r="C32" s="16"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="18" t="s">
         <v>17</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D33" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="25" t="s">
+      <c r="E33" s="21" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="20"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="22" t="s">
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="25" t="s">
+      <c r="E35" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="16"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="18"/>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="16"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="16"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="16"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="20"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="22"/>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="20"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="22" t="s">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="16"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C45" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C46" s="16"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C47" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C48" s="16"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="20"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="20"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E43" s="25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="20"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="E45" s="25" t="s">
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C49" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="20"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="20"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D49" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="E49" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C50" s="20"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="22"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>